<commit_message>
Fix Gia Vat Lieu Xay Dung
</commit_message>
<xml_diff>
--- a/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGianuocsh.xlsx
+++ b/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGianuocsh.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AspNetCore\net5\CSDLGia\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A2ACA-AD36-4DCD-8A7D-C44B264CB2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBC70EF-0B3D-4A83-A93F-3DBF463C372F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,68 +25,263 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
-  <si>
-    <t>Mục đích sử dụng</t>
-  </si>
-  <si>
-    <t>Đơn giá</t>
-  </si>
-  <si>
-    <t>Nước sạch sinh hoạt</t>
-  </si>
-  <si>
-    <t>Năm áp dụng
-(1)</t>
-  </si>
-  <si>
-    <t>Giá tiền
-(1)</t>
-  </si>
-  <si>
-    <t>Năm áp dụng
-(2)</t>
-  </si>
-  <si>
-    <t>Giá tiền
-(2)</t>
-  </si>
-  <si>
-    <t>Năm áp dụng
-(3)</t>
-  </si>
-  <si>
-    <t>Giá tiền
-(4)</t>
-  </si>
-  <si>
-    <t>Năm áp dụng
-(5)</t>
-  </si>
-  <si>
-    <t>Giá tiền
-(3)</t>
-  </si>
-  <si>
-    <t>Năm áp dụng
-(4)</t>
-  </si>
-  <si>
-    <t>Giá tiền
-(5)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>MỤC ĐÍCH SỬ DỤNG</t>
+  </si>
+  <si>
+    <t>Tỷ trọng tiêu thụ (%)</t>
+  </si>
+  <si>
+    <t>Sản lượng</t>
+  </si>
+  <si>
+    <t>Đơn giá chưa bao gồm thuế GTGT</t>
+  </si>
+  <si>
+    <t>Đơn giá đã bao gồm thuế GTGT</t>
+  </si>
+  <si>
+    <t>(m3)</t>
+  </si>
+  <si>
+    <t>(đồng/m3)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>GIÁ TIÊU THỤ NƯỚC SẠCH BQ</t>
+  </si>
+  <si>
+    <t>Sinh hoạt hộ dân cư ( giá lũy tiến)</t>
+  </si>
+  <si>
+    <t>Hộ dân cư khu vực đô thị</t>
+  </si>
+  <si>
+    <r>
+      <t>Mức 10m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> đầu tiên (hộ/tháng)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Từ trên 10m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> đến 20m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (hộ/tháng)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Từ trên 20m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> đến 30m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (hộ/tháng)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Từ trên 30m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (hộ/tháng)</t>
+    </r>
+  </si>
+  <si>
+    <t>Hộ dân cư khu vực nông thôn</t>
+  </si>
+  <si>
+    <t>76,45%</t>
+  </si>
+  <si>
+    <t>12,13%</t>
+  </si>
+  <si>
+    <t>2,91%</t>
+  </si>
+  <si>
+    <t>2,87%</t>
+  </si>
+  <si>
+    <t>Các cơ quan HCSN</t>
+  </si>
+  <si>
+    <t>4,14%</t>
+  </si>
+  <si>
+    <t>Hoạt động sản xuất vật chất</t>
+  </si>
+  <si>
+    <t>1,05%</t>
+  </si>
+  <si>
+    <t>Kinh doanh dịch vụ</t>
+  </si>
+  <si>
+    <t>0,45%</t>
+  </si>
+  <si>
+    <t>Tổng</t>
+  </si>
+  <si>
+    <t>GIÁ NƯỚC SẠCH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -98,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,23 +301,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,119 +690,310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0BC2B6-4560-4170-B0EA-9A729F87B874}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="11" width="14" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>8441</v>
+      </c>
+      <c r="F4" s="4">
+        <v>8863</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="11">
+        <v>327064</v>
+      </c>
+      <c r="E12" s="11">
+        <v>7333</v>
+      </c>
+      <c r="F12" s="11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="11">
+        <v>51888</v>
+      </c>
+      <c r="E13" s="11">
+        <v>8429</v>
+      </c>
+      <c r="F13" s="11">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="11">
+        <v>12456</v>
+      </c>
+      <c r="E14" s="11">
+        <v>10095</v>
+      </c>
+      <c r="F14" s="11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="11">
+        <v>12258</v>
+      </c>
+      <c r="E15" s="11">
+        <v>10476</v>
+      </c>
+      <c r="F15" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>2</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11">
+        <v>17707</v>
+      </c>
+      <c r="E16" s="11">
+        <v>10095</v>
+      </c>
+      <c r="F16" s="11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="11">
+        <v>4507</v>
+      </c>
+      <c r="E17" s="11">
+        <v>12667</v>
+      </c>
+      <c r="F17" s="11">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1921</v>
+      </c>
+      <c r="E18" s="11">
+        <v>24762</v>
+      </c>
+      <c r="F18" s="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2022</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2023</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2024</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2025</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="J3" s="1">
-        <v>2026</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1000</v>
-      </c>
+      <c r="D19" s="9">
+        <v>427801</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>